<commit_message>
added snow crystale size plot
</commit_message>
<xml_diff>
--- a/snowpyt/data_example/20161216_snowpit.xlsx
+++ b/snowpyt/data_example/20161216_snowpit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t xml:space="preserve">Snowpit form for Snowpyt package</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t xml:space="preserve">East [deg]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">º</t>
   </si>
   <si>
     <t xml:space="preserve">North [deg]</t>
@@ -508,28 +505,31 @@
   </sheetPr>
   <dimension ref="A1:S66"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="1.48469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="1.48469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="1.75510204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="1.35204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="1.35204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="1.62244897959184"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,51 +775,47 @@
       <c r="B36" s="10" t="n">
         <v>7.52568333</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="C36" s="11"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="10" t="n">
         <v>60.5943166</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>41</v>
-      </c>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="10" t="n">
         <v>1214</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="10" t="n">
         <v>-8</v>
@@ -827,7 +823,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -840,71 +836,71 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
       <c r="L43" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
       <c r="O43" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
       <c r="R43" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="S43" s="7"/>
     </row>
     <row r="44" s="14" customFormat="true" ht="38.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="C44" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="D44" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="E44" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="F44" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="G44" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G44" s="12" t="s">
+      <c r="H44" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="H44" s="12" t="s">
+      <c r="I44" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="I44" s="12" t="s">
+      <c r="J44" s="12" t="s">
         <v>62</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>63</v>
       </c>
       <c r="K44" s="13"/>
       <c r="L44" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M44" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>65</v>
       </c>
       <c r="N44" s="12"/>
       <c r="O44" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="P44" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="P44" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="Q44" s="13"/>
       <c r="R44" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S44" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,7 +919,7 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J45" s="16" t="str">
         <f aca="false">IF(I45="feast",1,IF(I45="4 finger",2,IF(I45="3 finger",3,IF(I45="2 finger",4,IF(I45="1 finger",5,IF(I45="pencil",6,IF(I45="knife",7,IF(I45="nan","NaN","NaN"))))))))</f>
@@ -963,14 +959,14 @@
         <v>2</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J46" s="16" t="str">
         <f aca="false">IF(I46="feast",1,IF(I46="4 finger",2,IF(I46="3 finger",3,IF(I46="2 finger",4,IF(I46="1 finger",5,IF(I46="pencil",6,IF(I46="knife",7,IF(I46="nan","NaN","NaN"))))))))</f>
@@ -1013,7 +1009,7 @@
         <v>12</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F47" s="15"/>
       <c r="G47" s="15" t="n">
@@ -1023,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J47" s="16" t="str">
         <f aca="false">IF(I47="feast",1,IF(I47="4 finger",2,IF(I47="3 finger",3,IF(I47="2 finger",4,IF(I47="1 finger",5,IF(I47="pencil",6,IF(I47="knife",7,IF(I47="nan","NaN","NaN"))))))))</f>
@@ -1074,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J48" s="16" t="str">
         <f aca="false">IF(I48="feast",1,IF(I48="4 finger",2,IF(I48="3 finger",3,IF(I48="2 finger",4,IF(I48="1 finger",5,IF(I48="pencil",6,IF(I48="knife",7,IF(I48="nan","NaN","NaN"))))))))</f>
@@ -1125,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J49" s="16" t="str">
         <f aca="false">IF(I49="feast",1,IF(I49="4 finger",2,IF(I49="3 finger",3,IF(I49="2 finger",4,IF(I49="1 finger",5,IF(I49="pencil",6,IF(I49="knife",7,IF(I49="nan","NaN","NaN"))))))))</f>
@@ -1170,7 +1166,7 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J50" s="16" t="str">
         <f aca="false">IF(I50="feast",1,IF(I50="4 finger",2,IF(I50="3 finger",3,IF(I50="2 finger",4,IF(I50="1 finger",5,IF(I50="pencil",6,IF(I50="knife",7,IF(I50="nan","NaN","NaN"))))))))</f>
@@ -1223,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J51" s="16" t="str">
         <f aca="false">IF(I51="feast",1,IF(I51="4 finger",2,IF(I51="3 finger",3,IF(I51="2 finger",4,IF(I51="1 finger",5,IF(I51="pencil",6,IF(I51="knife",7,IF(I51="nan","NaN","NaN"))))))))</f>
@@ -1263,7 +1259,7 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
       <c r="I52" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J52" s="16" t="str">
         <f aca="false">IF(I52="feast",1,IF(I52="4 finger",2,IF(I52="3 finger",3,IF(I52="2 finger",4,IF(I52="1 finger",5,IF(I52="pencil",6,IF(I52="knife",7,IF(I52="nan","NaN","NaN"))))))))</f>
@@ -1311,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J53" s="16" t="str">
         <f aca="false">IF(I53="feast",1,IF(I53="4 finger",2,IF(I53="3 finger",3,IF(I53="2 finger",4,IF(I53="1 finger",5,IF(I53="pencil",6,IF(I53="knife",7,IF(I53="nan","NaN","NaN"))))))))</f>
@@ -1347,7 +1343,7 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J54" s="16" t="str">
         <f aca="false">IF(I54="feast",1,IF(I54="4 finger",2,IF(I54="3 finger",3,IF(I54="2 finger",4,IF(I54="1 finger",5,IF(I54="pencil",6,IF(I54="knife",7,IF(I54="nan","NaN","NaN"))))))))</f>
@@ -1391,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J55" s="16" t="str">
         <f aca="false">IF(I55="feast",1,IF(I55="4 finger",2,IF(I55="3 finger",3,IF(I55="2 finger",4,IF(I55="1 finger",5,IF(I55="pencil",6,IF(I55="knife",7,IF(I55="nan","NaN","NaN"))))))))</f>
@@ -1423,7 +1419,7 @@
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J56" s="16" t="str">
         <f aca="false">IF(I56="feast",1,IF(I56="4 finger",2,IF(I56="3 finger",3,IF(I56="2 finger",4,IF(I56="1 finger",5,IF(I56="pencil",6,IF(I56="knife",7,IF(I56="nan","NaN","NaN"))))))))</f>
@@ -1463,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J57" s="16" t="str">
         <f aca="false">IF(I57="feast",1,IF(I57="4 finger",2,IF(I57="3 finger",3,IF(I57="2 finger",4,IF(I57="1 finger",5,IF(I57="pencil",6,IF(I57="knife",7,IF(I57="nan","NaN","NaN"))))))))</f>
@@ -1495,7 +1491,7 @@
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J58" s="16" t="str">
         <f aca="false">IF(I58="feast",1,IF(I58="4 finger",2,IF(I58="3 finger",3,IF(I58="2 finger",4,IF(I58="1 finger",5,IF(I58="pencil",6,IF(I58="knife",7,IF(I58="nan","NaN","NaN"))))))))</f>
@@ -1535,7 +1531,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J59" s="16" t="str">
         <f aca="false">IF(I59="feast",1,IF(I59="4 finger",2,IF(I59="3 finger",3,IF(I59="2 finger",4,IF(I59="1 finger",5,IF(I59="pencil",6,IF(I59="knife",7,IF(I59="nan","NaN","NaN"))))))))</f>
@@ -1561,7 +1557,7 @@
         <v>4</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J60" s="16" t="str">
         <f aca="false">IF(I60="feast",1,IF(I60="4 finger",2,IF(I60="3 finger",3,IF(I60="2 finger",4,IF(I60="1 finger",5,IF(I60="pencil",6,IF(I60="knife",7,IF(I60="nan","NaN","NaN"))))))))</f>
@@ -1592,7 +1588,7 @@
         <v>0.5</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J61" s="16" t="str">
         <f aca="false">IF(I61="feast",1,IF(I61="4 finger",2,IF(I61="3 finger",3,IF(I61="2 finger",4,IF(I61="1 finger",5,IF(I61="pencil",6,IF(I61="knife",7,IF(I61="nan","NaN","NaN"))))))))</f>
@@ -1619,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J62" s="16" t="str">
         <f aca="false">IF(I62="feast",1,IF(I62="4 finger",2,IF(I62="3 finger",3,IF(I62="2 finger",4,IF(I62="1 finger",5,IF(I62="pencil",6,IF(I62="knife",7,IF(I62="nan","NaN","NaN"))))))))</f>
@@ -1650,7 +1646,7 @@
         <v>0.5</v>
       </c>
       <c r="I63" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J63" s="16" t="str">
         <f aca="false">IF(I63="feast",1,IF(I63="4 finger",2,IF(I63="3 finger",3,IF(I63="2 finger",4,IF(I63="1 finger",5,IF(I63="pencil",6,IF(I63="knife",7,IF(I63="nan","NaN","NaN"))))))))</f>
@@ -1668,7 +1664,7 @@
         <v>27</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
@@ -1679,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J64" s="16" t="str">
         <f aca="false">IF(I64="feast",1,IF(I64="4 finger",2,IF(I64="3 finger",3,IF(I64="2 finger",4,IF(I64="1 finger",5,IF(I64="pencil",6,IF(I64="knife",7,IF(I64="nan","NaN","NaN"))))))))</f>
@@ -1697,7 +1693,7 @@
         <v>38</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
@@ -1708,7 +1704,7 @@
         <v>4</v>
       </c>
       <c r="I65" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J65" s="16" t="str">
         <f aca="false">IF(I65="feast",1,IF(I65="4 finger",2,IF(I65="3 finger",3,IF(I65="2 finger",4,IF(I65="1 finger",5,IF(I65="pencil",6,IF(I65="knife",7,IF(I65="nan","NaN","NaN"))))))))</f>
@@ -1733,7 +1729,7 @@
       <c r="G66" s="15"/>
       <c r="H66" s="15"/>
       <c r="I66" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J66" s="16" t="str">
         <f aca="false">IF(I66="feast",1,IF(I66="4 finger",2,IF(I66="3 finger",3,IF(I66="2 finger",4,IF(I66="1 finger",5,IF(I66="pencil",6,IF(I66="knife",7,IF(I66="nan","NaN","NaN"))))))))</f>

</xml_diff>